<commit_message>
Modified the criteria for MS diagnosis related to MS pregnancy cohort entry date
</commit_message>
<xml_diff>
--- a/i_codebooks/D3_DU_PREGNANCY_COHORT_variables.xlsx
+++ b/i_codebooks/D3_DU_PREGNANCY_COHORT_variables.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20406"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rosgin2\Documents\DP3-MS-SLE\i_codebooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lol\Documents\DP3-MS-SLE\i_codebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B832D2D2-38D0-4EE9-8480-7F01A157BA9F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8784"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8784" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -425,13 +426,6 @@
     <t>Whether woman develops MS during or right after this pregnancy</t>
   </si>
   <si>
-    <t xml:space="preserve">in DS with complete data this variable is 1 if
-pregnancy_with_MS_detail == "before  pregnancy"
-in THL and EFEMERIS this variable is 1 if
-pregnancy_with_MS_detail == "before  pregnancy" | pregnancy_with_MS_detail == "right before  pregnancy" (TO BE DECIDED: case when pregnancy_with_MS_detail == "during  pregnancy", and what about 'right after pregnancy'?)
-</t>
-  </si>
-  <si>
     <t>pregnancy_with_MS_detail != "no" &amp; pregnancy_with_MS == 0 (check case right after pregnancy)</t>
   </si>
   <si>
@@ -480,11 +474,18 @@
   <si>
     <t>this needs to be adapted a bit across data sources??</t>
   </si>
+  <si>
+    <t xml:space="preserve">in DS with complete data (SAIL, FERRARA and UOSL) this variable is 1 if
+pregnancy_with_MS_detail == "long before  pregnancy"
+in THL, Fisabio and EFEMERIS this variable is 1 if
+pregnancy_with_MS_detail == "long before  pregnancy" | pregnancy_with_MS_detail == "right before  pregnancy" |  pregnancy_with_MS_detail == "recently before  pregnancy" |pregnancy_with_MS_detail == "during  pregnancy"
+</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
@@ -589,7 +590,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -617,6 +618,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -922,9 +929,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -940,9 +944,12 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1154,14 +1161,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="32.6640625" customWidth="1"/>
     <col min="2" max="2" width="144.6640625" customWidth="1"/>
@@ -4218,22 +4225,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K976"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B31" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="E11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A9" sqref="A9:D40"/>
+      <selection pane="bottomRight" activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="31.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43.109375" style="41" customWidth="1"/>
     <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="44.33203125" customWidth="1"/>
+    <col min="4" max="4" width="55.33203125" customWidth="1"/>
     <col min="5" max="5" width="13.33203125" customWidth="1"/>
     <col min="6" max="6" width="31.6640625" style="41" customWidth="1"/>
     <col min="7" max="7" width="25.21875" customWidth="1"/>
@@ -4475,13 +4482,13 @@
         <v>46</v>
       </c>
       <c r="B13" s="41" t="s">
+        <v>138</v>
+      </c>
+      <c r="F13" s="57" t="s">
+        <v>140</v>
+      </c>
+      <c r="G13" s="53" t="s">
         <v>139</v>
-      </c>
-      <c r="F13" s="58" t="s">
-        <v>141</v>
-      </c>
-      <c r="G13" s="53" t="s">
-        <v>140</v>
       </c>
       <c r="H13" t="s">
         <v>23</v>
@@ -4493,7 +4500,7 @@
         <v>48</v>
       </c>
       <c r="B14" s="45" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C14" s="44" t="s">
         <v>60</v>
@@ -4509,7 +4516,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="216">
+    <row r="15" spans="1:11" ht="201.6">
       <c r="A15" s="44" t="s">
         <v>62</v>
       </c>
@@ -4518,17 +4525,17 @@
       </c>
       <c r="C15" s="44"/>
       <c r="D15" s="49" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E15" s="46"/>
       <c r="F15" s="41" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I15" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="K15" s="60" t="s">
-        <v>144</v>
+      <c r="K15" s="59" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="144">
@@ -4541,15 +4548,15 @@
       <c r="C16" s="44" t="s">
         <v>60</v>
       </c>
-      <c r="D16" s="56" t="s">
+      <c r="D16" s="55" t="s">
         <v>126</v>
       </c>
       <c r="E16" s="46"/>
       <c r="I16" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="K16" s="55" t="s">
-        <v>131</v>
+      <c r="K16" s="60" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="28.8">
@@ -4562,15 +4569,15 @@
       <c r="C17" s="44" t="s">
         <v>60</v>
       </c>
-      <c r="D17" s="56" t="s">
+      <c r="D17" s="55" t="s">
         <v>128</v>
       </c>
       <c r="E17" s="46"/>
       <c r="I17" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="K17" s="57" t="s">
-        <v>132</v>
+      <c r="K17" s="56" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="34.799999999999997" customHeight="1">
@@ -4642,16 +4649,16 @@
     </row>
     <row r="22" spans="1:11" ht="72">
       <c r="A22" s="43" t="s">
+        <v>134</v>
+      </c>
+      <c r="B22" s="41" t="s">
         <v>135</v>
       </c>
-      <c r="B22" s="41" t="s">
-        <v>136</v>
-      </c>
       <c r="C22" s="43" t="s">
+        <v>132</v>
+      </c>
+      <c r="D22" s="48" t="s">
         <v>133</v>
-      </c>
-      <c r="D22" s="48" t="s">
-        <v>134</v>
       </c>
       <c r="F22" s="41" t="s">
         <v>71</v>
@@ -4660,7 +4667,7 @@
         <v>23</v>
       </c>
       <c r="K22" s="43" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="28.8">
@@ -4873,7 +4880,7 @@
       <c r="C33" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="F33" s="59" t="s">
+      <c r="F33" s="58" t="s">
         <v>110</v>
       </c>
       <c r="I33" s="53" t="s">
@@ -4893,7 +4900,7 @@
       <c r="C34" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="F34" s="59" t="s">
+      <c r="F34" s="58" t="s">
         <v>110</v>
       </c>
       <c r="I34" s="53" t="s">
@@ -4913,7 +4920,7 @@
       <c r="C35" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="F35" s="59" t="s">
+      <c r="F35" s="58" t="s">
         <v>118</v>
       </c>
       <c r="I35" s="53" t="s">
@@ -4933,7 +4940,7 @@
       <c r="C36" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="F36" s="59" t="s">
+      <c r="F36" s="58" t="s">
         <v>118</v>
       </c>
       <c r="I36" s="53" t="s">
@@ -5966,12 +5973,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="37.6640625" customWidth="1"/>
     <col min="2" max="2" width="33.33203125" customWidth="1"/>
@@ -6990,14 +6997,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:L12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="8.6640625" customWidth="1"/>
     <col min="2" max="3" width="11.109375" customWidth="1"/>

</xml_diff>

<commit_message>
Modifications born during programming of template 3
</commit_message>
<xml_diff>
--- a/i_codebooks/D3_DU_PREGNANCY_COHORT_variables.xlsx
+++ b/i_codebooks/D3_DU_PREGNANCY_COHORT_variables.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20406"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20407"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Davide\Documents\Git repositories\Work\DP3-MS-SLE - Copy\i_codebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43E2E2B5-5BDF-456F-A475-F01B0DB98C33}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A1E7D57-6E37-45CA-931B-D59A701103BC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8790" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="145">
   <si>
     <t>medatata_name</t>
   </si>
@@ -355,15 +355,6 @@
     <t>end_preg_period_during_2</t>
   </si>
   <si>
-    <t>min(pregnancy_start_date + 195, pregnancy_end_date)</t>
-  </si>
-  <si>
-    <t>min(pregnancy_start_date + 98, pregnancy_end_date)</t>
-  </si>
-  <si>
-    <t>if pregnancy ends before day 98, is this missing?</t>
-  </si>
-  <si>
     <t>start_preg_period_during_3</t>
   </si>
   <si>
@@ -382,12 +373,6 @@
     <t>date when the period "Third trimester of pregnancy" ends (see table 5 page 12 of the SAP)</t>
   </si>
   <si>
-    <t>min(pregnancy_start_date + 196, pregnancy_end_date)</t>
-  </si>
-  <si>
-    <t>if pregnancy ends before day 196, is this missing?</t>
-  </si>
-  <si>
     <t>start_preg_period_after_1</t>
   </si>
   <si>
@@ -404,9 +389,6 @@
   </si>
   <si>
     <t>pregnancy_end_date + 90</t>
-  </si>
-  <si>
-    <t>interval in days between the previous pregnancy and this one</t>
   </si>
   <si>
     <t>1 = pregnancy with MS
@@ -478,6 +460,31 @@
     <t>t1 = pregnacy ended in first trimester
 t2 = pregnacy ended in second trimester
 t3 = pregnacy ended in third trimester</t>
+  </si>
+  <si>
+    <t>interval in months between the previous pregnancy and this one</t>
+  </si>
+  <si>
+    <t>fifelse(end_preg_period_during_1 != pregnancy_end_date,
+                                                            pregnancy_start_date %m+% days(98), NA)</t>
+  </si>
+  <si>
+    <t>fifelse(end_preg_period_during_1 != pregnancy_end_date,
+                                                          pmin(pregnancy_start_date %m+% days(195), pregnancy_end_date), NA)</t>
+  </si>
+  <si>
+    <t>fifelse(!is.na(end_preg_period_during_2) &amp; end_preg_period_during_2 != pregnancy_end_date,
+                                                            pregnancy_start_date %m+% days(196), NA)</t>
+  </si>
+  <si>
+    <t>fifelse(!is.na(end_preg_period_during_2) &amp; end_preg_period_during_2 != pregnancy_end_date,
+                                                          pregnancy_end_date, NA)</t>
+  </si>
+  <si>
+    <t>if pregnancy ends before day 98, this is missing</t>
+  </si>
+  <si>
+    <t>if pregnancy ends before day 196, this is missing</t>
   </si>
 </sst>
 </file>
@@ -939,7 +946,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -966,6 +972,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4247,11 +4256,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z975"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B32" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="E17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D40" sqref="D40"/>
+      <selection pane="bottomRight" activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -4501,13 +4510,13 @@
         <v>46</v>
       </c>
       <c r="B13" s="41" t="s">
-        <v>134</v>
-      </c>
-      <c r="F13" s="56" t="s">
-        <v>136</v>
+        <v>128</v>
+      </c>
+      <c r="F13" s="55" t="s">
+        <v>130</v>
       </c>
       <c r="G13" s="53" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="H13" t="s">
         <v>23</v>
@@ -4519,7 +4528,7 @@
         <v>48</v>
       </c>
       <c r="B14" s="45" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="C14" s="44" t="s">
         <v>60</v>
@@ -4544,17 +4553,17 @@
       </c>
       <c r="C15" s="44"/>
       <c r="D15" s="49" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="E15" s="46"/>
       <c r="F15" s="41" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="I15" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="K15" s="58" t="s">
-        <v>139</v>
+      <c r="K15" s="57" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="150">
@@ -4567,15 +4576,15 @@
       <c r="C16" s="44" t="s">
         <v>60</v>
       </c>
-      <c r="D16" s="55" t="s">
-        <v>126</v>
+      <c r="D16" s="54" t="s">
+        <v>120</v>
       </c>
       <c r="E16" s="46"/>
       <c r="I16" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="K16" s="59" t="s">
-        <v>140</v>
+      <c r="K16" s="58" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="34.9" customHeight="1">
@@ -4630,7 +4639,7 @@
         <v>68</v>
       </c>
       <c r="B20" s="41" t="s">
-        <v>125</v>
+        <v>138</v>
       </c>
       <c r="C20" s="43" t="s">
         <v>58</v>
@@ -4647,16 +4656,16 @@
     </row>
     <row r="21" spans="1:11" ht="75">
       <c r="A21" s="43" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B21" s="41" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="C21" s="43" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="D21" s="48" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="F21" s="41" t="s">
         <v>71</v>
@@ -4665,7 +4674,7 @@
         <v>23</v>
       </c>
       <c r="K21" s="43" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="45">
@@ -4679,7 +4688,7 @@
         <v>29</v>
       </c>
       <c r="F22" s="41" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="I22" s="53" t="s">
         <v>23</v>
@@ -4699,7 +4708,7 @@
         <v>29</v>
       </c>
       <c r="F23" s="41" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="I23" s="53" t="s">
         <v>23</v>
@@ -4719,7 +4728,7 @@
         <v>29</v>
       </c>
       <c r="F24" s="41" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="I24" s="53" t="s">
         <v>23</v>
@@ -4739,7 +4748,7 @@
         <v>29</v>
       </c>
       <c r="F25" s="41" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="I25" s="53" t="s">
         <v>23</v>
@@ -4759,7 +4768,7 @@
         <v>29</v>
       </c>
       <c r="F26" s="41" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="I26" s="53" t="s">
         <v>23</v>
@@ -4779,7 +4788,7 @@
         <v>29</v>
       </c>
       <c r="F27" s="41" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="I27" s="53" t="s">
         <v>23</v>
@@ -4799,7 +4808,7 @@
         <v>29</v>
       </c>
       <c r="F28" s="41" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="I28" s="53" t="s">
         <v>23</v>
@@ -4819,7 +4828,7 @@
         <v>29</v>
       </c>
       <c r="F29" s="41" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="I29" s="53" t="s">
         <v>23</v>
@@ -4839,7 +4848,7 @@
         <v>29</v>
       </c>
       <c r="F30" s="41" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="I30" s="53" t="s">
         <v>23</v>
@@ -4859,7 +4868,7 @@
         <v>29</v>
       </c>
       <c r="F31" s="41" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="I31" s="53" t="s">
         <v>23</v>
@@ -4873,19 +4882,19 @@
         <v>106</v>
       </c>
       <c r="B32" s="41" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C32" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="F32" s="57" t="s">
-        <v>110</v>
+      <c r="F32" s="56" t="s">
+        <v>143</v>
       </c>
       <c r="I32" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="K32" s="54" t="s">
-        <v>109</v>
+      <c r="K32" s="64" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="33" spans="1:26" ht="45">
@@ -4893,99 +4902,99 @@
         <v>107</v>
       </c>
       <c r="B33" s="41" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C33" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="F33" s="57" t="s">
-        <v>110</v>
+      <c r="F33" s="56" t="s">
+        <v>143</v>
       </c>
       <c r="I33" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="K33" s="54" t="s">
+      <c r="K33" s="64" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="34" spans="1:26" ht="60">
+      <c r="A34" s="43" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="34" spans="1:26" ht="45">
-      <c r="A34" s="43" t="s">
-        <v>111</v>
-      </c>
       <c r="B34" s="41" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C34" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="F34" s="57" t="s">
-        <v>118</v>
+      <c r="F34" s="56" t="s">
+        <v>144</v>
       </c>
       <c r="I34" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="K34" s="54" t="s">
-        <v>117</v>
+      <c r="K34" s="64" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="35" spans="1:26" ht="45">
       <c r="A35" s="43" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B35" s="41" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C35" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="F35" s="57" t="s">
-        <v>118</v>
+      <c r="F35" s="56" t="s">
+        <v>144</v>
       </c>
       <c r="I35" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="K35" s="54" t="s">
-        <v>35</v>
+      <c r="K35" s="64" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="36" spans="1:26" ht="45">
       <c r="A36" s="43" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B36" s="41" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C36" s="43" t="s">
         <v>29</v>
       </c>
       <c r="F36" s="41" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="I36" s="53" t="s">
         <v>23</v>
       </c>
       <c r="K36" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="37" spans="1:26" ht="45">
       <c r="A37" s="43" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B37" s="41" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C37" s="43" t="s">
         <v>29</v>
       </c>
       <c r="F37" s="41" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="I37" s="53" t="s">
         <v>23</v>
       </c>
       <c r="K37" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="38" spans="1:26" ht="45">
@@ -4999,7 +5008,7 @@
         <v>29</v>
       </c>
       <c r="F38" s="41" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="I38" s="53" t="s">
         <v>23</v>
@@ -5019,7 +5028,7 @@
         <v>29</v>
       </c>
       <c r="F39" s="41" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="I39" s="53" t="s">
         <v>23</v>
@@ -5029,38 +5038,38 @@
       </c>
     </row>
     <row r="40" spans="1:26" ht="36">
-      <c r="A40" s="60" t="s">
-        <v>141</v>
-      </c>
-      <c r="B40" s="61"/>
-      <c r="C40" s="62" t="s">
-        <v>142</v>
-      </c>
-      <c r="D40" s="63" t="s">
-        <v>143</v>
-      </c>
-      <c r="E40" s="63"/>
+      <c r="A40" s="59" t="s">
+        <v>135</v>
+      </c>
+      <c r="B40" s="60"/>
+      <c r="C40" s="61" t="s">
+        <v>136</v>
+      </c>
+      <c r="D40" s="62" t="s">
+        <v>137</v>
+      </c>
+      <c r="E40" s="62"/>
       <c r="F40" s="6"/>
-      <c r="G40" s="64"/>
-      <c r="H40" s="64"/>
-      <c r="I40" s="64"/>
-      <c r="J40" s="64"/>
-      <c r="K40" s="64"/>
-      <c r="L40" s="64"/>
-      <c r="M40" s="64"/>
-      <c r="N40" s="64"/>
-      <c r="O40" s="64"/>
-      <c r="P40" s="64"/>
-      <c r="Q40" s="64"/>
-      <c r="R40" s="64"/>
-      <c r="S40" s="64"/>
-      <c r="T40" s="64"/>
-      <c r="U40" s="64"/>
-      <c r="V40" s="64"/>
-      <c r="W40" s="64"/>
-      <c r="X40" s="64"/>
-      <c r="Y40" s="64"/>
-      <c r="Z40" s="64"/>
+      <c r="G40" s="63"/>
+      <c r="H40" s="63"/>
+      <c r="I40" s="63"/>
+      <c r="J40" s="63"/>
+      <c r="K40" s="63"/>
+      <c r="L40" s="63"/>
+      <c r="M40" s="63"/>
+      <c r="N40" s="63"/>
+      <c r="O40" s="63"/>
+      <c r="P40" s="63"/>
+      <c r="Q40" s="63"/>
+      <c r="R40" s="63"/>
+      <c r="S40" s="63"/>
+      <c r="T40" s="63"/>
+      <c r="U40" s="63"/>
+      <c r="V40" s="63"/>
+      <c r="W40" s="63"/>
+      <c r="X40" s="63"/>
+      <c r="Y40" s="63"/>
+      <c r="Z40" s="63"/>
     </row>
     <row r="41" spans="1:26" ht="15.75" customHeight="1"/>
     <row r="42" spans="1:26" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Updated codebooks and documentation website
</commit_message>
<xml_diff>
--- a/i_codebooks/D3_DU_PREGNANCY_COHORT_variables.xlsx
+++ b/i_codebooks/D3_DU_PREGNANCY_COHORT_variables.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20407"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20410"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Davide\Documents\Git repositories\Work\DP3-MS-SLE - Copy\i_codebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A1E7D57-6E37-45CA-931B-D59A701103BC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F85F707B-1E7E-4EB2-9E03-FA6C726EBC54}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8790" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="146">
   <si>
     <t>medatata_name</t>
   </si>
@@ -247,15 +247,9 @@
     <t>missing if has_previous_pregnancy != 1</t>
   </si>
   <si>
-    <t>pregnancy_start_date - pregnancy_end_date[previous pregnancy of the same person]</t>
-  </si>
-  <si>
     <t>start_preg_period_pre_all</t>
   </si>
   <si>
-    <t>pregnancy_start_date - 365</t>
-  </si>
-  <si>
     <t>end_preg_period_pre_all</t>
   </si>
   <si>
@@ -280,9 +274,6 @@
     <t>date when the period "9-12 months before pregnancy" ends (see table 5 page 12 of the SAP)</t>
   </si>
   <si>
-    <t>pregnancy_start_date - 275</t>
-  </si>
-  <si>
     <t>start_preg_period_pre_2</t>
   </si>
   <si>
@@ -317,21 +308,6 @@
   </si>
   <si>
     <t>date when the period "0-3 months before pregnancy" ends (see table 5 page 12 of the SAP)</t>
-  </si>
-  <si>
-    <t>pregnancy_start_date - 274</t>
-  </si>
-  <si>
-    <t>pregnancy_start_date - 183</t>
-  </si>
-  <si>
-    <t>pregnancy_start_date - 182</t>
-  </si>
-  <si>
-    <t>pregnancy_start_date - 91</t>
-  </si>
-  <si>
-    <t>pregnancy_start_date - 90</t>
   </si>
   <si>
     <t>start_preg_period_during_1</t>
@@ -412,9 +388,6 @@
   </si>
   <si>
     <t>categories of interval between the previous pregnancy and this one</t>
-  </si>
-  <si>
-    <t>categorise time_since_previous_pregnancy</t>
   </si>
   <si>
     <t>Whether woman has MS ever during the study period</t>
@@ -485,6 +458,45 @@
   </si>
   <si>
     <t>if pregnancy ends before day 196, this is missing</t>
+  </si>
+  <si>
+    <t>categorise time_since_previous_pregnancy
+(a,b]</t>
+  </si>
+  <si>
+    <t>ceiling(pregnancy_start_date - pregnancy_end_date[previous pregnancy of the same person] / 30.4)</t>
+  </si>
+  <si>
+    <t>pregnancy_start_date - 365
+Missing in datasources with only pregnancies</t>
+  </si>
+  <si>
+    <t>pregnancy_start_date - 275
+Missing in datasources with only pregnancies</t>
+  </si>
+  <si>
+    <t>pregnancy_start_date - 274
+Missing in datasources with only pregnancies</t>
+  </si>
+  <si>
+    <t>pregnancy_start_date - 183
+Missing in datasources with only pregnancies</t>
+  </si>
+  <si>
+    <t>pregnancy_start_date - 182
+Missing in datasources with only pregnancies</t>
+  </si>
+  <si>
+    <t>pregnancy_start_date - 91
+Missing in datasources with only pregnancies</t>
+  </si>
+  <si>
+    <t>pregnancy_start_date - 90
+in EFEMERIS 78 days are used instead</t>
+  </si>
+  <si>
+    <t>start_preg_period_pre_4
+start_preg_period_pre_1 in datasources with only pregnancies</t>
   </si>
 </sst>
 </file>
@@ -494,11 +506,25 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -811,145 +837,145 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -961,20 +987,24 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4256,11 +4286,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z975"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E17" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="G34" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F37" sqref="F37"/>
+      <selection pane="bottomRight" activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -4510,13 +4540,13 @@
         <v>46</v>
       </c>
       <c r="B13" s="41" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="F13" s="55" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="G13" s="53" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="H13" t="s">
         <v>23</v>
@@ -4528,7 +4558,7 @@
         <v>48</v>
       </c>
       <c r="B14" s="45" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="C14" s="44" t="s">
         <v>60</v>
@@ -4553,17 +4583,17 @@
       </c>
       <c r="C15" s="44"/>
       <c r="D15" s="49" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="E15" s="46"/>
       <c r="F15" s="41" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="I15" s="42" t="s">
         <v>23</v>
       </c>
       <c r="K15" s="57" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="150">
@@ -4577,14 +4607,14 @@
         <v>60</v>
       </c>
       <c r="D16" s="54" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="E16" s="46"/>
       <c r="I16" s="42" t="s">
         <v>23</v>
       </c>
       <c r="K16" s="58" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="34.9" customHeight="1">
@@ -4639,7 +4669,7 @@
         <v>68</v>
       </c>
       <c r="B20" s="41" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="C20" s="43" t="s">
         <v>58</v>
@@ -4650,22 +4680,22 @@
       <c r="I20" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="K20" t="s">
-        <v>72</v>
+      <c r="K20" s="66" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="75">
       <c r="A21" s="43" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="B21" s="41" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="C21" s="43" t="s">
-        <v>122</v>
-      </c>
-      <c r="D21" s="48" t="s">
-        <v>123</v>
+        <v>114</v>
+      </c>
+      <c r="D21" s="65" t="s">
+        <v>115</v>
       </c>
       <c r="F21" s="41" t="s">
         <v>71</v>
@@ -4674,181 +4704,181 @@
         <v>23</v>
       </c>
       <c r="K21" s="43" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="45">
       <c r="A22" s="43" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B22" s="41" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C22" s="43" t="s">
         <v>29</v>
       </c>
       <c r="F22" s="41" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="I22" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="K22" t="s">
-        <v>74</v>
+      <c r="K22" s="48" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="45">
       <c r="A23" s="43" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B23" s="41" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C23" s="43" t="s">
         <v>29</v>
       </c>
       <c r="F23" s="41" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="I23" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="K23" t="s">
-        <v>83</v>
+      <c r="K23" s="48" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="45">
       <c r="A24" s="43" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B24" s="41" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C24" s="43" t="s">
         <v>29</v>
       </c>
       <c r="F24" s="41" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="I24" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="K24" t="s">
-        <v>96</v>
+      <c r="K24" s="48" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="45">
       <c r="A25" s="43" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B25" s="41" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C25" s="43" t="s">
         <v>29</v>
       </c>
       <c r="F25" s="41" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="I25" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="K25" t="s">
-        <v>97</v>
+      <c r="K25" s="48" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="45">
       <c r="A26" s="43" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B26" s="41" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C26" s="43" t="s">
         <v>29</v>
       </c>
       <c r="F26" s="41" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="I26" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="K26" t="s">
-        <v>98</v>
+      <c r="K26" s="48" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="45">
       <c r="A27" s="43" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B27" s="41" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C27" s="43" t="s">
         <v>29</v>
       </c>
       <c r="F27" s="41" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="I27" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="K27" t="s">
-        <v>99</v>
+      <c r="K27" s="48" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="45">
       <c r="A28" s="43" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B28" s="41" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C28" s="43" t="s">
         <v>29</v>
       </c>
       <c r="F28" s="41" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="I28" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="K28" t="s">
-        <v>100</v>
+      <c r="K28" s="48" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="45">
       <c r="A29" s="43" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B29" s="41" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C29" s="43" t="s">
         <v>29</v>
       </c>
       <c r="F29" s="41" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="I29" s="53" t="s">
         <v>23</v>
       </c>
       <c r="K29" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="45">
       <c r="A30" s="43" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="B30" s="41" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="C30" s="43" t="s">
         <v>29</v>
       </c>
       <c r="F30" s="41" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="I30" s="53" t="s">
         <v>23</v>
@@ -4859,194 +4889,194 @@
     </row>
     <row r="31" spans="1:11" ht="45">
       <c r="A31" s="43" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B31" s="41" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="C31" s="43" t="s">
         <v>29</v>
       </c>
       <c r="F31" s="41" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="I31" s="53" t="s">
         <v>23</v>
       </c>
       <c r="K31" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="45">
       <c r="A32" s="43" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="B32" s="41" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="C32" s="43" t="s">
         <v>29</v>
       </c>
       <c r="F32" s="56" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="I32" s="53" t="s">
         <v>23</v>
       </c>
       <c r="K32" s="64" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
     </row>
     <row r="33" spans="1:26" ht="45">
       <c r="A33" s="43" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="B33" s="41" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C33" s="43" t="s">
         <v>29</v>
       </c>
       <c r="F33" s="56" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="I33" s="53" t="s">
         <v>23</v>
       </c>
       <c r="K33" s="64" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
     </row>
     <row r="34" spans="1:26" ht="60">
       <c r="A34" s="43" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B34" s="41" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="C34" s="43" t="s">
         <v>29</v>
       </c>
       <c r="F34" s="56" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="I34" s="53" t="s">
         <v>23</v>
       </c>
       <c r="K34" s="64" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
     </row>
     <row r="35" spans="1:26" ht="45">
       <c r="A35" s="43" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="B35" s="41" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="C35" s="43" t="s">
         <v>29</v>
       </c>
       <c r="F35" s="56" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="I35" s="53" t="s">
         <v>23</v>
       </c>
       <c r="K35" s="64" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
     </row>
     <row r="36" spans="1:26" ht="45">
       <c r="A36" s="43" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="B36" s="41" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="C36" s="43" t="s">
         <v>29</v>
       </c>
       <c r="F36" s="41" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="I36" s="53" t="s">
         <v>23</v>
       </c>
       <c r="K36" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
     </row>
     <row r="37" spans="1:26" ht="45">
       <c r="A37" s="43" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="B37" s="41" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C37" s="43" t="s">
         <v>29</v>
       </c>
       <c r="F37" s="41" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="I37" s="53" t="s">
         <v>23</v>
       </c>
       <c r="K37" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
     </row>
     <row r="38" spans="1:26" ht="45">
       <c r="A38" s="43" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B38" s="41" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C38" s="43" t="s">
         <v>29</v>
       </c>
       <c r="F38" s="41" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="I38" s="53" t="s">
         <v>23</v>
       </c>
       <c r="K38" s="43" t="s">
-        <v>90</v>
+        <v>145</v>
       </c>
     </row>
     <row r="39" spans="1:26" ht="45">
       <c r="A39" s="43" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B39" s="41" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C39" s="43" t="s">
         <v>29</v>
       </c>
       <c r="F39" s="41" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="I39" s="53" t="s">
         <v>23</v>
       </c>
       <c r="K39" s="43" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="40" spans="1:26" ht="36">
       <c r="A40" s="59" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="B40" s="60"/>
       <c r="C40" s="61" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="D40" s="62" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E40" s="62"/>
       <c r="F40" s="6"/>

</xml_diff>

<commit_message>
Trying to remove commas
</commit_message>
<xml_diff>
--- a/i_codebooks/D3_DU_PREGNANCY_COHORT_variables.xlsx
+++ b/i_codebooks/D3_DU_PREGNANCY_COHORT_variables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Davide\Documents\Git repositories\Work\DP3-MS-SLE - Copy\i_codebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85EEFCF4-BB45-4E80-9894-83869B890690}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C3F66EC-ECA7-4348-9997-003A11BCD43E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8790" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8790" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -256,24 +256,12 @@
     <t>pregnancy_start_date - 1</t>
   </si>
   <si>
-    <t>date when the period "12 months before pregnancy" starts (see table 5 page 12 of the SAP)</t>
-  </si>
-  <si>
-    <t>date when the period "12 months before pregnancy" ends (see table 5 page 12 of the SAP)</t>
-  </si>
-  <si>
-    <t>date when the period "9-12 months before pregnancy" starts (see table 5 page 12 of the SAP)</t>
-  </si>
-  <si>
     <t>end_preg_period_pre_3</t>
   </si>
   <si>
     <t>start_preg_period_pre_3</t>
   </si>
   <si>
-    <t>date when the period "9-12 months before pregnancy" ends (see table 5 page 12 of the SAP)</t>
-  </si>
-  <si>
     <t>start_preg_period_pre_2</t>
   </si>
   <si>
@@ -286,42 +274,18 @@
     <t>end_preg_period_pre_1</t>
   </si>
   <si>
-    <t>date when the period "6-9 months before pregnancy" starts (see table 5 page 12 of the SAP)</t>
-  </si>
-  <si>
-    <t>date when the period "6-9 months before pregnancy" ends (see table 5 page 12 of the SAP)</t>
-  </si>
-  <si>
     <t>start_preg_period_pre_4</t>
   </si>
   <si>
     <t>end_preg_period_pre_4</t>
   </si>
   <si>
-    <t>date when the period "3-6 months before pregnancy" starts (see table 5 page 12 of the SAP)</t>
-  </si>
-  <si>
-    <t>date when the period "3-6 months before pregnancy" ends (see table 5 page 12 of the SAP)</t>
-  </si>
-  <si>
-    <t>date when the period "0-3 months before pregnancy" starts (see table 5 page 12 of the SAP)</t>
-  </si>
-  <si>
-    <t>date when the period "0-3 months before pregnancy" ends (see table 5 page 12 of the SAP)</t>
-  </si>
-  <si>
     <t>start_preg_period_during_1</t>
   </si>
   <si>
     <t>end_preg_period_during_1</t>
   </si>
   <si>
-    <t>date when the period "First trimester of pregnancy" starts (see table 5 page 12 of the SAP)</t>
-  </si>
-  <si>
-    <t>date when the period "First trimester of pregnancy" ends (see table 5 page 12 of the SAP)</t>
-  </si>
-  <si>
     <t>min(pregnancy_start_date + 97, pregnancy_end_date)</t>
   </si>
   <si>
@@ -337,28 +301,10 @@
     <t>end_preg_period_during_3</t>
   </si>
   <si>
-    <t>date when the period "Second trimester of pregnancy" starts (see table 5 page 12 of the SAP)</t>
-  </si>
-  <si>
-    <t>date when the period "Second trimester of pregnancy" ends (see table 5 page 12 of the SAP)</t>
-  </si>
-  <si>
-    <t>date when the period "Third trimester of pregnancy" starts (see table 5 page 12 of the SAP)</t>
-  </si>
-  <si>
-    <t>date when the period "Third trimester of pregnancy" ends (see table 5 page 12 of the SAP)</t>
-  </si>
-  <si>
     <t>start_preg_period_after_1</t>
   </si>
   <si>
     <t>end_preg_period_after_1</t>
-  </si>
-  <si>
-    <t>date when the period "0-3 months after pregnancy" starts (see table 5 page 12 of the SAP)</t>
-  </si>
-  <si>
-    <t>date when the period "0-3 months after pregnancy" ends (see table 5 page 12 of the SAP)</t>
   </si>
   <si>
     <t>pregnancy_end_date + 1</t>
@@ -405,23 +351,7 @@
     <t>See Figure 3 of the SAP. This is missing if has_MS_ever!= 1</t>
   </si>
   <si>
-    <t xml:space="preserve">"long after pregnancy" = MS diagnosed after DU_pregnancy_study_exit_date
-"right after pregnancy" = MS diagnosed between pregnancy_end_date and DU_pregnancy_study_exit_date
-"during pregnancy" = MS diagnosed between pregnancy_start_date and pregnancy_end_date
-"right before pregnancy" = MS diagnosed between 3 months before pregnancy and pregnancy_start_date
-"recently before pregnancy" = MS diagnosed between DU_pregnancy_study_entry_date and 3 months before pregnancy 
-"long before pregnancy" = MS diagnosed before DU_pregnancy_study_entry_date
-</t>
-  </si>
-  <si>
     <t>this needs to be adapted a bit across data sources??</t>
-  </si>
-  <si>
-    <t xml:space="preserve">in DS with complete data (SAIL, FERRARA and UOSL) this variable is 1 if
-pregnancy_with_MS_detail == "long before  pregnancy"
-in THL, Fisabio and EFEMERIS this variable is 1 if
-pregnancy_with_MS_detail == "long before  pregnancy" | pregnancy_with_MS_detail == "right before  pregnancy" |  pregnancy_with_MS_detail == "recently before  pregnancy" |pregnancy_with_MS_detail == "during  pregnancy"
-</t>
   </si>
   <si>
     <t>trimester_when_pregnancy_ended</t>
@@ -500,6 +430,76 @@
   </si>
   <si>
     <t>empty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">long after pregnancy = MS diagnosed after DU_pregnancy_study_exit_date
+right after pregnancy = MS diagnosed between pregnancy_end_date and DU_pregnancy_study_exit_date
+during pregnancy = MS diagnosed between pregnancy_start_date and pregnancy_end_date
+right before pregnancy = MS diagnosed between 3 months before pregnancy and pregnancy_start_date
+recently before pregnancy = MS diagnosed between DU_pregnancy_study_entry_date and 3 months before pregnancy 
+long before pregnancy = MS diagnosed before DU_pregnancy_study_entry_date
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">in DS with complete data (SAIL, FERRARA and UOSL) this variable is 1 if
+pregnancy_with_MS_detail == long before  pregnancy
+in THL, Fisabio and EFEMERIS this variable is 1 if
+pregnancy_with_MS_detail == long before  pregnancy | pregnancy_with_MS_detail == right before  pregnancy |  pregnancy_with_MS_detail == recently before  pregnancy |pregnancy_with_MS_detail == during  pregnancy
+</t>
+  </si>
+  <si>
+    <t>date when the period 9-12 months before pregnancy starts (see table 5 page 12 of the SAP)</t>
+  </si>
+  <si>
+    <t>date when the period 9-12 months before pregnancy ends (see table 5 page 12 of the SAP)</t>
+  </si>
+  <si>
+    <t>date when the period 6-9 months before pregnancy starts (see table 5 page 12 of the SAP)</t>
+  </si>
+  <si>
+    <t>date when the period 6-9 months before pregnancy ends (see table 5 page 12 of the SAP)</t>
+  </si>
+  <si>
+    <t>date when the period 3-6 months before pregnancy starts (see table 5 page 12 of the SAP)</t>
+  </si>
+  <si>
+    <t>date when the period 3-6 months before pregnancy ends (see table 5 page 12 of the SAP)</t>
+  </si>
+  <si>
+    <t>date when the period 0-3 months before pregnancy starts (see table 5 page 12 of the SAP)</t>
+  </si>
+  <si>
+    <t>date when the period 0-3 months before pregnancy ends (see table 5 page 12 of the SAP)</t>
+  </si>
+  <si>
+    <t>date when the period First trimester of pregnancy starts (see table 5 page 12 of the SAP)</t>
+  </si>
+  <si>
+    <t>date when the period First trimester of pregnancy ends (see table 5 page 12 of the SAP)</t>
+  </si>
+  <si>
+    <t>date when the period Second trimester of pregnancy starts (see table 5 page 12 of the SAP)</t>
+  </si>
+  <si>
+    <t>date when the period Second trimester of pregnancy ends (see table 5 page 12 of the SAP)</t>
+  </si>
+  <si>
+    <t>date when the period Third trimester of pregnancy starts (see table 5 page 12 of the SAP)</t>
+  </si>
+  <si>
+    <t>date when the period Third trimester of pregnancy ends (see table 5 page 12 of the SAP)</t>
+  </si>
+  <si>
+    <t>date when the period 0-3 months after pregnancy starts (see table 5 page 12 of the SAP)</t>
+  </si>
+  <si>
+    <t>date when the period 0-3 months after pregnancy ends (see table 5 page 12 of the SAP)</t>
+  </si>
+  <si>
+    <t>date when the period 12 months before pregnancy starts (see table 5 page 12 of the SAP)</t>
+  </si>
+  <si>
+    <t>date when the period 12 months before pregnancy ends (see table 5 page 12 of the SAP)</t>
   </si>
 </sst>
 </file>
@@ -509,11 +509,18 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -847,145 +854,145 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -997,25 +1004,28 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4297,11 +4307,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z975"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="G34" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K38" sqref="K38"/>
+      <selection pane="bottomRight" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -4551,13 +4561,13 @@
         <v>46</v>
       </c>
       <c r="B13" s="41" t="s">
-        <v>119</v>
+        <v>101</v>
       </c>
       <c r="F13" s="55" t="s">
-        <v>121</v>
+        <v>103</v>
       </c>
       <c r="G13" s="53" t="s">
-        <v>120</v>
+        <v>102</v>
       </c>
       <c r="H13" t="s">
         <v>23</v>
@@ -4569,7 +4579,7 @@
         <v>48</v>
       </c>
       <c r="B14" s="45" t="s">
-        <v>118</v>
+        <v>100</v>
       </c>
       <c r="C14" s="44" t="s">
         <v>60</v>
@@ -4594,17 +4604,17 @@
       </c>
       <c r="C15" s="44"/>
       <c r="D15" s="49" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="E15" s="46"/>
       <c r="F15" s="41" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
       <c r="I15" s="42" t="s">
         <v>23</v>
       </c>
       <c r="K15" s="57" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="150">
@@ -4618,14 +4628,14 @@
         <v>60</v>
       </c>
       <c r="D16" s="54" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="E16" s="46"/>
       <c r="I16" s="42" t="s">
         <v>23</v>
       </c>
       <c r="K16" s="58" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="34.9" customHeight="1">
@@ -4680,7 +4690,7 @@
         <v>68</v>
       </c>
       <c r="B20" s="41" t="s">
-        <v>129</v>
+        <v>109</v>
       </c>
       <c r="C20" s="43" t="s">
         <v>58</v>
@@ -4692,21 +4702,21 @@
         <v>23</v>
       </c>
       <c r="K20" s="66" t="s">
-        <v>137</v>
+        <v>117</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="75">
       <c r="A21" s="43" t="s">
-        <v>116</v>
+        <v>98</v>
       </c>
       <c r="B21" s="41" t="s">
-        <v>117</v>
+        <v>99</v>
       </c>
       <c r="C21" s="43" t="s">
-        <v>114</v>
+        <v>96</v>
       </c>
       <c r="D21" s="65" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
       <c r="F21" s="41" t="s">
         <v>71</v>
@@ -4715,161 +4725,161 @@
         <v>23</v>
       </c>
       <c r="K21" s="43" t="s">
-        <v>136</v>
+        <v>116</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="45">
       <c r="A22" s="43" t="s">
-        <v>87</v>
-      </c>
-      <c r="B22" s="41" t="s">
-        <v>77</v>
+        <v>81</v>
+      </c>
+      <c r="B22" s="68" t="s">
+        <v>129</v>
       </c>
       <c r="C22" s="43" t="s">
         <v>29</v>
       </c>
       <c r="F22" s="41" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="I22" s="53" t="s">
         <v>23</v>
       </c>
       <c r="K22" s="48" t="s">
-        <v>138</v>
+        <v>118</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="45">
       <c r="A23" s="43" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B23" s="41" t="s">
-        <v>80</v>
+        <v>130</v>
       </c>
       <c r="C23" s="43" t="s">
         <v>29</v>
       </c>
       <c r="F23" s="41" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="I23" s="53" t="s">
         <v>23</v>
       </c>
       <c r="K23" s="48" t="s">
-        <v>139</v>
+        <v>119</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="45">
       <c r="A24" s="43" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B24" s="41" t="s">
-        <v>85</v>
+        <v>131</v>
       </c>
       <c r="C24" s="43" t="s">
         <v>29</v>
       </c>
       <c r="F24" s="41" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="I24" s="53" t="s">
         <v>23</v>
       </c>
       <c r="K24" s="48" t="s">
-        <v>140</v>
+        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="45">
       <c r="A25" s="43" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B25" s="41" t="s">
-        <v>86</v>
+        <v>132</v>
       </c>
       <c r="C25" s="43" t="s">
         <v>29</v>
       </c>
       <c r="F25" s="41" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="I25" s="53" t="s">
         <v>23</v>
       </c>
       <c r="K25" s="48" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="45">
       <c r="A26" s="43" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B26" s="41" t="s">
-        <v>89</v>
+        <v>133</v>
       </c>
       <c r="C26" s="43" t="s">
         <v>29</v>
       </c>
       <c r="F26" s="41" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="I26" s="53" t="s">
         <v>23</v>
       </c>
       <c r="K26" s="48" t="s">
-        <v>142</v>
+        <v>122</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="45">
       <c r="A27" s="43" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B27" s="41" t="s">
-        <v>90</v>
+        <v>134</v>
       </c>
       <c r="C27" s="43" t="s">
         <v>29</v>
       </c>
       <c r="F27" s="41" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="I27" s="53" t="s">
         <v>23</v>
       </c>
       <c r="K27" s="48" t="s">
-        <v>143</v>
+        <v>123</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="45">
       <c r="A28" s="43" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B28" s="41" t="s">
-        <v>91</v>
+        <v>135</v>
       </c>
       <c r="C28" s="43" t="s">
         <v>29</v>
       </c>
       <c r="F28" s="41" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="I28" s="53" t="s">
         <v>23</v>
       </c>
       <c r="K28" s="48" t="s">
-        <v>144</v>
+        <v>124</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="45">
       <c r="A29" s="43" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B29" s="41" t="s">
-        <v>92</v>
+        <v>136</v>
       </c>
       <c r="C29" s="43" t="s">
         <v>29</v>
       </c>
       <c r="F29" s="41" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="I29" s="53" t="s">
         <v>23</v>
@@ -4880,16 +4890,16 @@
     </row>
     <row r="30" spans="1:11" ht="45">
       <c r="A30" s="43" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="B30" s="41" t="s">
-        <v>95</v>
+        <v>137</v>
       </c>
       <c r="C30" s="43" t="s">
         <v>29</v>
       </c>
       <c r="F30" s="41" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="I30" s="53" t="s">
         <v>23</v>
@@ -4900,142 +4910,142 @@
     </row>
     <row r="31" spans="1:11" ht="45">
       <c r="A31" s="43" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="B31" s="41" t="s">
-        <v>96</v>
+        <v>138</v>
       </c>
       <c r="C31" s="43" t="s">
         <v>29</v>
       </c>
       <c r="F31" s="41" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="I31" s="53" t="s">
         <v>23</v>
       </c>
       <c r="K31" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="45">
       <c r="A32" s="43" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="B32" s="41" t="s">
-        <v>102</v>
+        <v>139</v>
       </c>
       <c r="C32" s="43" t="s">
         <v>29</v>
       </c>
       <c r="F32" s="56" t="s">
-        <v>134</v>
+        <v>114</v>
       </c>
       <c r="I32" s="53" t="s">
         <v>23</v>
       </c>
       <c r="K32" s="64" t="s">
-        <v>130</v>
+        <v>110</v>
       </c>
     </row>
     <row r="33" spans="1:26" ht="45">
       <c r="A33" s="43" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="B33" s="41" t="s">
-        <v>103</v>
+        <v>140</v>
       </c>
       <c r="C33" s="43" t="s">
         <v>29</v>
       </c>
       <c r="F33" s="56" t="s">
-        <v>134</v>
+        <v>114</v>
       </c>
       <c r="I33" s="53" t="s">
         <v>23</v>
       </c>
       <c r="K33" s="64" t="s">
-        <v>131</v>
+        <v>111</v>
       </c>
     </row>
     <row r="34" spans="1:26" ht="60">
       <c r="A34" s="43" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="B34" s="41" t="s">
-        <v>104</v>
+        <v>141</v>
       </c>
       <c r="C34" s="43" t="s">
         <v>29</v>
       </c>
       <c r="F34" s="56" t="s">
-        <v>135</v>
+        <v>115</v>
       </c>
       <c r="I34" s="53" t="s">
         <v>23</v>
       </c>
       <c r="K34" s="64" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
     </row>
     <row r="35" spans="1:26" ht="45">
       <c r="A35" s="43" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="B35" s="41" t="s">
-        <v>105</v>
+        <v>142</v>
       </c>
       <c r="C35" s="43" t="s">
         <v>29</v>
       </c>
       <c r="F35" s="56" t="s">
-        <v>135</v>
+        <v>115</v>
       </c>
       <c r="I35" s="53" t="s">
         <v>23</v>
       </c>
       <c r="K35" s="64" t="s">
-        <v>133</v>
+        <v>113</v>
       </c>
     </row>
     <row r="36" spans="1:26" ht="45">
       <c r="A36" s="43" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="B36" s="41" t="s">
-        <v>108</v>
+        <v>143</v>
       </c>
       <c r="C36" s="43" t="s">
         <v>29</v>
       </c>
       <c r="F36" s="41" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="I36" s="53" t="s">
         <v>23</v>
       </c>
       <c r="K36" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
     </row>
     <row r="37" spans="1:26" ht="45">
       <c r="A37" s="43" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="B37" s="41" t="s">
-        <v>109</v>
+        <v>144</v>
       </c>
       <c r="C37" s="43" t="s">
         <v>29</v>
       </c>
       <c r="F37" s="41" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="I37" s="53" t="s">
         <v>23</v>
       </c>
       <c r="K37" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
     </row>
     <row r="38" spans="1:26" ht="45">
@@ -5043,19 +5053,19 @@
         <v>72</v>
       </c>
       <c r="B38" s="41" t="s">
-        <v>75</v>
+        <v>145</v>
       </c>
       <c r="C38" s="43" t="s">
         <v>29</v>
       </c>
       <c r="F38" s="41" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="I38" s="53" t="s">
         <v>23</v>
       </c>
       <c r="K38" s="43" t="s">
-        <v>145</v>
+        <v>125</v>
       </c>
     </row>
     <row r="39" spans="1:26" ht="45">
@@ -5063,31 +5073,31 @@
         <v>73</v>
       </c>
       <c r="B39" s="41" t="s">
-        <v>76</v>
+        <v>146</v>
       </c>
       <c r="C39" s="43" t="s">
         <v>29</v>
       </c>
       <c r="F39" s="41" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="I39" s="53" t="s">
         <v>23</v>
       </c>
       <c r="K39" s="43" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="40" spans="1:26" ht="36">
       <c r="A40" s="59" t="s">
-        <v>126</v>
+        <v>106</v>
       </c>
       <c r="B40" s="60"/>
       <c r="C40" s="61" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
       <c r="D40" s="62" t="s">
-        <v>128</v>
+        <v>108</v>
       </c>
       <c r="E40" s="62"/>
       <c r="F40" s="6"/>
@@ -6047,7 +6057,7 @@
     <row r="975" ht="15.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7079,7 +7089,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -7093,7 +7103,7 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="67" t="s">
-        <v>146</v>
+        <v>126</v>
       </c>
       <c r="B1" s="34"/>
       <c r="C1" s="1"/>

</xml_diff>

<commit_message>
Test for longer tables
</commit_message>
<xml_diff>
--- a/i_codebooks/D3_DU_PREGNANCY_COHORT_variables.xlsx
+++ b/i_codebooks/D3_DU_PREGNANCY_COHORT_variables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Davide\Documents\Git repositories\Work\DP3-MS-SLE - Copy\i_codebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C3F66EC-ECA7-4348-9997-003A11BCD43E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48771727-EF0D-45DC-9384-BF3F24B794D8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8790" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8790" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -429,9 +429,6 @@
 start_preg_period_pre_1 in datasources with only pregnancies</t>
   </si>
   <si>
-    <t>empty</t>
-  </si>
-  <si>
     <t xml:space="preserve">long after pregnancy = MS diagnosed after DU_pregnancy_study_exit_date
 right after pregnancy = MS diagnosed between pregnancy_end_date and DU_pregnancy_study_exit_date
 during pregnancy = MS diagnosed between pregnancy_start_date and pregnancy_end_date
@@ -500,6 +497,9 @@
   </si>
   <si>
     <t>date when the period 12 months before pregnancy ends (see table 5 page 12 of the SAP)</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -1022,10 +1022,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4307,7 +4307,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z975"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -4604,7 +4604,7 @@
       </c>
       <c r="C15" s="44"/>
       <c r="D15" s="49" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E15" s="46"/>
       <c r="F15" s="41" t="s">
@@ -4635,7 +4635,7 @@
         <v>23</v>
       </c>
       <c r="K16" s="58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="34.9" customHeight="1">
@@ -4732,8 +4732,8 @@
       <c r="A22" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="B22" s="68" t="s">
-        <v>129</v>
+      <c r="B22" s="67" t="s">
+        <v>128</v>
       </c>
       <c r="C22" s="43" t="s">
         <v>29</v>
@@ -4753,7 +4753,7 @@
         <v>82</v>
       </c>
       <c r="B23" s="41" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C23" s="43" t="s">
         <v>29</v>
@@ -4773,7 +4773,7 @@
         <v>76</v>
       </c>
       <c r="B24" s="41" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C24" s="43" t="s">
         <v>29</v>
@@ -4793,7 +4793,7 @@
         <v>75</v>
       </c>
       <c r="B25" s="41" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C25" s="43" t="s">
         <v>29</v>
@@ -4813,7 +4813,7 @@
         <v>77</v>
       </c>
       <c r="B26" s="41" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C26" s="43" t="s">
         <v>29</v>
@@ -4833,7 +4833,7 @@
         <v>78</v>
       </c>
       <c r="B27" s="41" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C27" s="43" t="s">
         <v>29</v>
@@ -4853,7 +4853,7 @@
         <v>79</v>
       </c>
       <c r="B28" s="41" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C28" s="43" t="s">
         <v>29</v>
@@ -4873,7 +4873,7 @@
         <v>80</v>
       </c>
       <c r="B29" s="41" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C29" s="43" t="s">
         <v>29</v>
@@ -4893,7 +4893,7 @@
         <v>83</v>
       </c>
       <c r="B30" s="41" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C30" s="43" t="s">
         <v>29</v>
@@ -4913,7 +4913,7 @@
         <v>84</v>
       </c>
       <c r="B31" s="41" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C31" s="43" t="s">
         <v>29</v>
@@ -4933,7 +4933,7 @@
         <v>86</v>
       </c>
       <c r="B32" s="41" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C32" s="43" t="s">
         <v>29</v>
@@ -4953,7 +4953,7 @@
         <v>87</v>
       </c>
       <c r="B33" s="41" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C33" s="43" t="s">
         <v>29</v>
@@ -4973,7 +4973,7 @@
         <v>88</v>
       </c>
       <c r="B34" s="41" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C34" s="43" t="s">
         <v>29</v>
@@ -4993,7 +4993,7 @@
         <v>89</v>
       </c>
       <c r="B35" s="41" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C35" s="43" t="s">
         <v>29</v>
@@ -5013,7 +5013,7 @@
         <v>90</v>
       </c>
       <c r="B36" s="41" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C36" s="43" t="s">
         <v>29</v>
@@ -5033,7 +5033,7 @@
         <v>91</v>
       </c>
       <c r="B37" s="41" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C37" s="43" t="s">
         <v>29</v>
@@ -5053,7 +5053,7 @@
         <v>72</v>
       </c>
       <c r="B38" s="41" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C38" s="43" t="s">
         <v>29</v>
@@ -5073,7 +5073,7 @@
         <v>73</v>
       </c>
       <c r="B39" s="41" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C39" s="43" t="s">
         <v>29</v>
@@ -7089,7 +7089,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -7102,8 +7102,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="67" t="s">
-        <v>126</v>
+      <c r="A1" s="68" t="s">
+        <v>146</v>
       </c>
       <c r="B1" s="34"/>
       <c r="C1" s="1"/>

</xml_diff>